<commit_message>
feat:Message Alarm - modify table
need to display alarms on top.jsp
</commit_message>
<xml_diff>
--- a/src/main/resources/com/config/나랑노랑_테이블정의.xlsx
+++ b/src/main/resources/com/config/나랑노랑_테이블정의.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaeyen\git\NarangNorang\src\main\resources\com\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EC4BA2-C7A6-48F2-845E-BED01F68E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F80ECA-8DFB-426E-A004-9438A7D54B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9870" yWindow="450" windowWidth="16080" windowHeight="15150" activeTab="2" xr2:uid="{FEBEA036-6C71-4209-BF10-49EF14142D6B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="163">
   <si>
     <t>엔티티타입명</t>
   </si>
@@ -663,6 +663,10 @@
   </si>
   <si>
     <t>READ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFAULT 0 NOT NULL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2201,7 +2205,7 @@
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2415,7 +2419,7 @@
         <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
@@ -3162,6 +3166,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:H3"/>
@@ -3170,11 +3179,6 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:H11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3786,13 +3790,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:H20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="I17:J17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:H3"/>
@@ -3801,6 +3798,13 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:H12"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:H20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>